<commit_message>
updating test for changes to wc_utils.workbook
</commit_message>
<xml_diff>
--- a/tests/fixtures/uncaught-error.xlsx
+++ b/tests/fixtures/uncaught-error.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main root" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,8 +16,10 @@
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Tests!$A$1:$C$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Main root'!$A$1:$B$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Main root'!$A$1:$B$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Main root'!$A$1:$B$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Tests!$A$1:$C$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Tests!$A$1:$C$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Tests!$A$1:$C$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,45 +31,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>€</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Float1</t>
-  </si>
-  <si>
-    <t>Bool1</t>
-  </si>
-  <si>
-    <t>node_0</t>
-  </si>
-  <si>
-    <t>node_1</t>
-  </si>
-  <si>
-    <t>node_2</t>
-  </si>
-  <si>
-    <t>node_3</t>
-  </si>
-  <si>
-    <t>node_4</t>
-  </si>
-  <si>
-    <t>'</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">Identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Float1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bool1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">node_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">node_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">node_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">node_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">node_4</t>
   </si>
 </sst>
 </file>
@@ -75,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
   </numFmts>
   <fonts count="6">
@@ -182,7 +184,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,12 +279,12 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -326,7 +328,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -383,26 +385,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>0</v>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>